<commit_message>
Work until 2123 2101014
</commit_message>
<xml_diff>
--- a/Data/Phase Diagram Data.xlsx
+++ b/Data/Phase Diagram Data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Dropbox\Workspace\Github\CZTS-Project\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="285" windowWidth="21075" windowHeight="7725" activeTab="2"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="600K" sheetId="2" r:id="rId2"/>
     <sheet name="900K" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -402,6 +407,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -449,7 +457,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -484,7 +492,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3377,8 +3385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>